<commit_message>
Finalize workshop and send to editing.
</commit_message>
<xml_diff>
--- a/development/output/worksheet_03.xlsx
+++ b/development/output/worksheet_03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Employee Company Overview Information</t>
   </si>
@@ -38,6 +38,78 @@
   </si>
   <si>
     <t>Maryland</t>
+  </si>
+  <si>
+    <t>Employee Status</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>On Leave</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Avg YOS</t>
+  </si>
+  <si>
+    <t>EXECUTIVE</t>
+  </si>
+  <si>
+    <t>PUBLICATIONS</t>
+  </si>
+  <si>
+    <t>VIDEO</t>
+  </si>
+  <si>
+    <t>INTERNAL DATA BASE</t>
+  </si>
+  <si>
+    <t>TEXAS REGIONAL</t>
+  </si>
+  <si>
+    <t>FINANCE</t>
+  </si>
+  <si>
+    <t>CALIFORNIA REGIONAL</t>
+  </si>
+  <si>
+    <t>SOFTWARE DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>SALES &amp; MARKETING</t>
+  </si>
+  <si>
+    <t>QUALITY ASSURANCE</t>
+  </si>
+  <si>
+    <t>HUMAN RESOURCES</t>
+  </si>
+  <si>
+    <t>HOST SYSTEMS DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>CONTRACTS</t>
+  </si>
+  <si>
+    <t>DOCUMENTATION DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>FACILITIES</t>
+  </si>
+  <si>
+    <t>EDUCATION</t>
+  </si>
+  <si>
+    <t>INFORMATION SYSTEMS</t>
+  </si>
+  <si>
+    <t>TECHNICAL SUPPORT</t>
+  </si>
+  <si>
+    <t>CORPORATE COMMUNICATIONS</t>
   </si>
 </sst>
 </file>
@@ -239,6 +311,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>510064</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" title="The SGPlot Procedure" descr="The SGPlot Procedure"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>510064</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" title="The SGPlot Procedure" descr="The SGPlot Procedure"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -361,7 +509,7 @@
   <sheetPr filterMode="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
     </sheetView>
@@ -433,6 +581,194 @@
     </row>
     <row r="40" ht="20" customHeight="1"/>
     <row r="71" ht="20" customHeight="1"/>
+    <row r="72" ht="20" customHeight="1">
+      <c r="A72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" ht="20" customHeight="1">
+      <c r="A73" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="5">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="74" ht="20" customHeight="1">
+      <c r="A74" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" ht="20" customHeight="1"/>
+    <row r="112" ht="20" customHeight="1"/>
+    <row r="113" ht="20" customHeight="1">
+      <c r="A113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" ht="20" customHeight="1">
+      <c r="A114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="115" ht="20" customHeight="1">
+      <c r="A115" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B115" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" ht="20" customHeight="1">
+      <c r="A116" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B116" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" ht="20" customHeight="1">
+      <c r="A117" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" ht="20" customHeight="1">
+      <c r="A118" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" ht="20" customHeight="1">
+      <c r="A119" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B119" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" ht="20" customHeight="1">
+      <c r="A120" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B120" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" ht="20" customHeight="1">
+      <c r="A121" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" ht="20" customHeight="1">
+      <c r="A122" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B122" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" ht="20" customHeight="1">
+      <c r="A123" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B123" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" ht="20" customHeight="1">
+      <c r="A124" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" ht="20" customHeight="1">
+      <c r="A125" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B125" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" ht="20" customHeight="1">
+      <c r="A126" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B126" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" ht="20" customHeight="1">
+      <c r="A127" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" ht="20" customHeight="1">
+      <c r="A128" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B128" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" ht="20" customHeight="1">
+      <c r="A129" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B129" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" ht="20" customHeight="1">
+      <c r="A130" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B130" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" ht="20" customHeight="1">
+      <c r="A131" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B131" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" ht="20" customHeight="1">
+      <c r="A132" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B132" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" ht="20" customHeight="1"/>
+    <row r="170" ht="20" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>